<commit_message>
train model with new features
</commit_message>
<xml_diff>
--- a/tracking/features.xlsx
+++ b/tracking/features.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="460" windowWidth="22740" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-60" yWindow="460" windowWidth="22740" windowHeight="15460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Original features" sheetId="1" r:id="rId1"/>
     <sheet name="related posts" sheetId="3" r:id="rId2"/>
     <sheet name="New features importance" sheetId="4" r:id="rId3"/>
+    <sheet name="new features importance2" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="225">
   <si>
     <t>#</t>
   </si>
@@ -686,6 +687,24 @@
   </si>
   <si>
     <t>XGboost_Features</t>
+  </si>
+  <si>
+    <t>car13_car15</t>
+  </si>
+  <si>
+    <t>avg_car13_on_car04</t>
+  </si>
+  <si>
+    <t>avg_car13_on_car01</t>
+  </si>
+  <si>
+    <t>avg_car13_on_car02</t>
+  </si>
+  <si>
+    <t>avg_car13_on_car09</t>
+  </si>
+  <si>
+    <t>avg_car13_on_car07</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1232,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2592,7 +2613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3284,4 +3305,489 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" style="34" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" s="33">
+        <v>0.101656934296827</v>
+      </c>
+      <c r="C2" s="33">
+        <v>6.6965699877092305E-2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" s="33">
+        <v>9.6344092634208303E-2</v>
+      </c>
+      <c r="C3" s="33">
+        <v>3.5123731326263001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="33">
+        <v>8.8698965442326402E-2</v>
+      </c>
+      <c r="C4" s="33">
+        <v>8.7695290226935799E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="33">
+        <v>8.4505237294001001E-2</v>
+      </c>
+      <c r="C5" s="33">
+        <v>4.6274122223489297E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="33">
+        <v>6.7088878201772104E-2</v>
+      </c>
+      <c r="C6" s="33">
+        <v>7.2806984199389302E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="33">
+        <v>6.2213766387722899E-2</v>
+      </c>
+      <c r="C7" s="33">
+        <v>3.01694099162454E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="33">
+        <v>4.5318318014859603E-2</v>
+      </c>
+      <c r="C8" s="33">
+        <v>5.6892335373348001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9" s="33">
+        <v>3.9305506223947399E-2</v>
+      </c>
+      <c r="C9" s="33">
+        <v>3.3818628755337601E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" s="33">
+        <v>3.3232462402815299E-2</v>
+      </c>
+      <c r="C10" s="33">
+        <v>2.4315454695201501E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="33">
+        <v>3.2483758386462801E-2</v>
+      </c>
+      <c r="C11" s="33">
+        <v>4.2713599675624998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="33">
+        <v>2.9993466073982299E-2</v>
+      </c>
+      <c r="C12" s="33">
+        <v>1.31523928992283E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="B13" s="33">
+        <v>2.7603053887888002E-2</v>
+      </c>
+      <c r="C13" s="33">
+        <v>4.73131359207309E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="33">
+        <v>2.52971077138569E-2</v>
+      </c>
+      <c r="C14" s="33">
+        <v>3.3438501792932201E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="33">
+        <v>2.3395824042367799E-2</v>
+      </c>
+      <c r="C15" s="33">
+        <v>2.1325122590945399E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="33">
+        <v>2.1389975640313301E-2</v>
+      </c>
+      <c r="C16" s="33">
+        <v>2.29469976305419E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" s="33">
+        <v>1.97792005363027E-2</v>
+      </c>
+      <c r="C17" s="33">
+        <v>4.3017701245549399E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="33">
+        <v>1.8332561813045101E-2</v>
+      </c>
+      <c r="C18" s="33">
+        <v>1.00987063012379E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="33">
+        <v>1.82159685046967E-2</v>
+      </c>
+      <c r="C19" s="33">
+        <v>1.03267824786812E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="33">
+        <v>1.71752669295837E-2</v>
+      </c>
+      <c r="C20" s="33">
+        <v>1.4482837267647399E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="B21" s="33">
+        <v>1.5341075746750499E-2</v>
+      </c>
+      <c r="C21" s="33">
+        <v>1.2645556949354399E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" s="33">
+        <v>1.3781024809619799E-2</v>
+      </c>
+      <c r="C22" s="33">
+        <v>1.8600879360373E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" s="33">
+        <v>1.1465591000674199E-2</v>
+      </c>
+      <c r="C23" s="33">
+        <v>2.5835962544823302E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="33">
+        <v>1.13724942097926E-2</v>
+      </c>
+      <c r="C24" s="33">
+        <v>1.0820947529808301E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="33">
+        <v>1.1337150692633E-2</v>
+      </c>
+      <c r="C25" s="33">
+        <v>1.7207080498219701E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="B26" s="33">
+        <v>1.1006266733819801E-2</v>
+      </c>
+      <c r="C26" s="33">
+        <v>2.6013355127279199E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="B27" s="33">
+        <v>9.6431304970415292E-3</v>
+      </c>
+      <c r="C27" s="33">
+        <v>2.63427984946972E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="33">
+        <v>9.3597726642553596E-3</v>
+      </c>
+      <c r="C28" s="33">
+        <v>2.7787280951837901E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="B29" s="33">
+        <v>7.9618701715402796E-3</v>
+      </c>
+      <c r="C29" s="33">
+        <v>2.1502515173401199E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" s="33">
+        <v>6.6362163637294497E-3</v>
+      </c>
+      <c r="C30" s="33">
+        <v>1.8765601044082099E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="33">
+        <v>6.6296047960354597E-3</v>
+      </c>
+      <c r="C31" s="33">
+        <v>8.0586916029953999E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="33">
+        <v>6.4159892816749702E-3</v>
+      </c>
+      <c r="C32" s="33">
+        <v>1.6180737699725001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="B33" s="33">
+        <v>5.9304580792587302E-3</v>
+      </c>
+      <c r="C33" s="33">
+        <v>9.4524904651486896E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="33">
+        <v>5.8070424355452597E-3</v>
+      </c>
+      <c r="C34" s="33">
+        <v>7.5518556531214802E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="B35" s="33">
+        <v>5.3690981965173398E-3</v>
+      </c>
+      <c r="C35" s="33">
+        <v>1.3431152671658999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B36" s="33">
+        <v>3.6175072691710698E-3</v>
+      </c>
+      <c r="C36" s="33">
+        <v>1.02127443899596E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="33">
+        <v>1.9417804630933999E-3</v>
+      </c>
+      <c r="C37" s="33">
+        <v>6.0947022972339402E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="B38" s="33">
+        <v>1.2060050678853701E-3</v>
+      </c>
+      <c r="C38" s="33">
+        <v>3.2944336741805099E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="B39" s="33">
+        <v>1.17362041850181E-3</v>
+      </c>
+      <c r="C39" s="33">
+        <v>2.5215088506227701E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="33">
+        <v>1.0738444852093001E-3</v>
+      </c>
+      <c r="C40" s="33">
+        <v>2.1540527869641801E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B41" s="33">
+        <v>7.6897910828771499E-4</v>
+      </c>
+      <c r="C41" s="33">
+        <v>2.1033691919767898E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="B42" s="33">
+        <v>1.3113308198388899E-4</v>
+      </c>
+      <c r="C42" s="33">
+        <v>5.4484864611446901E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new aggregated data files
</commit_message>
<xml_diff>
--- a/tracking/features.xlsx
+++ b/tracking/features.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="460" windowWidth="22740" windowHeight="15460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="3880" yWindow="460" windowWidth="22740" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Original features" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="226">
   <si>
     <t>#</t>
   </si>
@@ -599,15 +599,9 @@
     <t>whether claimed before?</t>
   </si>
   <si>
-    <t># of preivous insurance claims?</t>
-  </si>
-  <si>
     <t>age groups…??? (the higher ps_ind_03, the higher ps_ind_01; and insurance claim rate is higher on two sides)</t>
   </si>
   <si>
-    <t>single or married or divorced? (something related to marriage, different group has different distribution of ps_ind_01)</t>
-  </si>
-  <si>
     <t>regional information; (4*ps_reg_03)^2 maps nicely to 2 decimal points</t>
   </si>
   <si>
@@ -705,6 +699,15 @@
   </si>
   <si>
     <t>avg_car13_on_car07</t>
+  </si>
+  <si>
+    <t>single or married or divorced? (something related to marriage or gender, different group has different distribution of ps_ind_01)</t>
+  </si>
+  <si>
+    <t>ps_ind_14 = (ps_ind_10 + ps_ind_11 + ps_ind_12 + ps_ind_13)</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/c/porto-seguro-safe-driver-prediction/discussion/41907</t>
   </si>
 </sst>
 </file>
@@ -942,16 +945,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1232,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1374,7 +1377,7 @@
         <v>148</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1431,10 +1434,10 @@
       <c r="E9" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="40" t="s">
         <v>187</v>
       </c>
       <c r="H9" s="30" t="s">
@@ -1457,8 +1460,8 @@
       <c r="E10" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="36"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
@@ -1476,8 +1479,8 @@
       <c r="E11" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="36"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="40"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
@@ -1495,8 +1498,8 @@
       <c r="E12" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
@@ -1598,7 +1601,10 @@
         <v>155</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>189</v>
+        <v>224</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
@@ -1636,11 +1642,11 @@
       <c r="E19" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="G19" s="36" t="s">
-        <v>191</v>
+      <c r="G19" s="40" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1659,8 +1665,8 @@
       <c r="E20" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="35"/>
-      <c r="G20" s="36"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="40"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
@@ -1678,8 +1684,8 @@
       <c r="E21" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="35"/>
-      <c r="G21" s="36"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="14">
@@ -1701,7 +1707,7 @@
         <v>146</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1724,7 +1730,7 @@
         <v>148</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1747,7 +1753,7 @@
         <v>148</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H24" s="30" t="s">
         <v>176</v>
@@ -2036,7 +2042,7 @@
         <v>148</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H38" s="30" t="s">
         <v>171</v>
@@ -2624,33 +2630,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>197</v>
+      <c r="A1" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>195</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="40">
+      <c r="A2" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="38">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="C2" s="40">
+      <c r="C2" s="38">
         <v>0.05</v>
       </c>
       <c r="F2" s="32" t="s">
@@ -2664,13 +2670,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" s="40">
+      <c r="A3" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="38">
         <v>9.4E-2</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="38">
         <v>6.2E-2</v>
       </c>
       <c r="F3" s="32" t="s">
@@ -2684,17 +2690,17 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="B4" s="40">
+      <c r="A4" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="38">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="38">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G4" s="33">
         <v>8.6423581872367594E-2</v>
@@ -2704,17 +2710,17 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="38">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="38">
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G5" s="33">
         <v>8.5035924618113101E-2</v>
@@ -2724,13 +2730,13 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="38">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="38">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -2744,13 +2750,13 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="38">
         <v>5.5E-2</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="38">
         <v>2.3E-2</v>
       </c>
       <c r="F7" s="32" t="s">
@@ -2764,13 +2770,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="38">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="38">
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="F8" s="32" t="s">
@@ -2784,17 +2790,17 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="B9" s="40">
+      <c r="A9" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="38">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="38">
         <v>0.04</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G9" s="33">
         <v>4.8002730280756398E-2</v>
@@ -2804,13 +2810,13 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="40">
+      <c r="B10" s="38">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="38">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F10" s="32" t="s">
@@ -2824,13 +2830,13 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
-        <v>202</v>
-      </c>
-      <c r="B11" s="40">
+      <c r="A11" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="38">
         <v>3.1E-2</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="38">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="F11" s="32" t="s">
@@ -2844,13 +2850,13 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="B12" s="40">
+      <c r="A12" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" s="38">
         <v>3.1E-2</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="38">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="F12" s="32" t="s">
@@ -2864,17 +2870,17 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="38">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="38">
         <v>3.9E-2</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G13" s="33">
         <v>3.5271315369844798E-2</v>
@@ -2884,13 +2890,13 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="B14" s="40">
+      <c r="A14" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="38">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="C14" s="40">
+      <c r="C14" s="38">
         <v>5.5E-2</v>
       </c>
       <c r="F14" s="32" t="s">
@@ -2904,17 +2910,17 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="40">
+      <c r="B15" s="38">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="38">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G15" s="33">
         <v>2.16963002470833E-2</v>
@@ -2924,13 +2930,13 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="39" t="s">
-        <v>210</v>
-      </c>
-      <c r="B16" s="40">
+      <c r="A16" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="38">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="38">
         <v>0.03</v>
       </c>
       <c r="F16" s="32" t="s">
@@ -2944,13 +2950,13 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="39" t="s">
-        <v>206</v>
-      </c>
-      <c r="B17" s="40">
+      <c r="A17" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="38">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="38">
         <v>3.1E-2</v>
       </c>
       <c r="F17" s="32" t="s">
@@ -2964,13 +2970,13 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
-        <v>205</v>
-      </c>
-      <c r="B18" s="40">
+      <c r="A18" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" s="38">
         <v>0.02</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="38">
         <v>0.02</v>
       </c>
       <c r="F18" s="32" t="s">
@@ -2984,13 +2990,13 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
-        <v>204</v>
-      </c>
-      <c r="B19" s="40">
+      <c r="A19" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="38">
         <v>0.02</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="38">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="F19" s="32" t="s">
@@ -3004,13 +3010,13 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="40">
+      <c r="B20" s="38">
         <v>1.9E-2</v>
       </c>
-      <c r="C20" s="40">
+      <c r="C20" s="38">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="F20" s="32" t="s">
@@ -3024,17 +3030,17 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="40">
+      <c r="B21" s="38">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="C21" s="40">
+      <c r="C21" s="38">
         <v>1.2E-2</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G21" s="33">
         <v>1.2427598893924001E-2</v>
@@ -3044,13 +3050,13 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="38">
         <v>1.6E-2</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="38">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F22" s="32" t="s">
@@ -3064,13 +3070,13 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="40">
+      <c r="B23" s="38">
         <v>1.6E-2</v>
       </c>
-      <c r="C23" s="40">
+      <c r="C23" s="38">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="F23" s="32" t="s">
@@ -3084,17 +3090,17 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="39" t="s">
-        <v>207</v>
-      </c>
-      <c r="B24" s="40">
+      <c r="A24" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" s="38">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="38">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G24" s="33">
         <v>2.7725983405526701E-3</v>
@@ -3104,13 +3110,13 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="40">
+      <c r="B25" s="38">
         <v>1.2E-2</v>
       </c>
-      <c r="C25" s="40">
+      <c r="C25" s="38">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F25" s="32" t="s">
@@ -3124,13 +3130,13 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="40">
+      <c r="B26" s="38">
         <v>1.2E-2</v>
       </c>
-      <c r="C26" s="40">
+      <c r="C26" s="38">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F26" s="32" t="s">
@@ -3144,13 +3150,13 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="40">
+      <c r="B27" s="38">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C27" s="40">
+      <c r="C27" s="38">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F27" s="32" t="s">
@@ -3164,13 +3170,13 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="39" t="s">
-        <v>211</v>
-      </c>
-      <c r="B28" s="40">
+      <c r="A28" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="B28" s="38">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C28" s="40">
+      <c r="C28" s="38">
         <v>1.6E-2</v>
       </c>
       <c r="F28" s="32" t="s">
@@ -3184,13 +3190,13 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="39" t="s">
-        <v>209</v>
-      </c>
-      <c r="B29" s="40">
+      <c r="A29" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" s="38">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="38">
         <v>0.01</v>
       </c>
       <c r="F29" s="32" t="s">
@@ -3204,101 +3210,101 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="40">
+      <c r="B30" s="38">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C30" s="40">
+      <c r="C30" s="38">
         <v>1.4E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="40">
+      <c r="B31" s="38">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="C31" s="40">
+      <c r="C31" s="38">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="B32" s="38">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C32" s="38">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="B33" s="38">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C33" s="38">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="B32" s="40">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C32" s="40">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="39" t="s">
+      <c r="B34" s="38">
+        <v>2E-3</v>
+      </c>
+      <c r="C34" s="38">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="38">
+        <v>2E-3</v>
+      </c>
+      <c r="C35" s="38">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="B33" s="40">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C33" s="40">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="39" t="s">
+      <c r="B36" s="38">
+        <v>1E-3</v>
+      </c>
+      <c r="C36" s="38">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="38">
+        <v>0</v>
+      </c>
+      <c r="C37" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="B34" s="40">
-        <v>2E-3</v>
-      </c>
-      <c r="C34" s="40">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="40">
-        <v>2E-3</v>
-      </c>
-      <c r="C35" s="40">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="B36" s="40">
-        <v>1E-3</v>
-      </c>
-      <c r="C36" s="40">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="40">
+      <c r="B38" s="38">
         <v>0</v>
       </c>
-      <c r="C37" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="B38" s="40">
-        <v>0</v>
-      </c>
-      <c r="C38" s="40">
+      <c r="C38" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3311,7 +3317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3320,22 +3326,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
-        <v>217</v>
+      <c r="A1" s="35" t="s">
+        <v>215</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B2" s="33">
         <v>0.101656934296827</v>
@@ -3349,7 +3355,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B3" s="33">
         <v>9.6344092634208303E-2</v>
@@ -3371,7 +3377,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B5" s="33">
         <v>8.4505237294001001E-2</v>
@@ -3415,7 +3421,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B9" s="33">
         <v>3.9305506223947399E-2</v>
@@ -3426,7 +3432,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B10" s="33">
         <v>3.3232462402815299E-2</v>
@@ -3459,7 +3465,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B13" s="33">
         <v>2.7603053887888002E-2</v>
@@ -3481,7 +3487,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B15" s="33">
         <v>2.3395824042367799E-2</v>
@@ -3492,7 +3498,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B16" s="33">
         <v>2.1389975640313301E-2</v>
@@ -3503,7 +3509,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B17" s="33">
         <v>1.97792005363027E-2</v>
@@ -3536,7 +3542,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B20" s="33">
         <v>1.71752669295837E-2</v>
@@ -3547,7 +3553,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B21" s="33">
         <v>1.5341075746750499E-2</v>
@@ -3558,7 +3564,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B22" s="33">
         <v>1.3781024809619799E-2</v>
@@ -3569,7 +3575,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B23" s="33">
         <v>1.1465591000674199E-2</v>
@@ -3602,7 +3608,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B26" s="33">
         <v>1.1006266733819801E-2</v>
@@ -3613,7 +3619,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B27" s="33">
         <v>9.6431304970415292E-3</v>
@@ -3635,7 +3641,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B29" s="33">
         <v>7.9618701715402796E-3</v>
@@ -3646,7 +3652,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B30" s="33">
         <v>6.6362163637294497E-3</v>
@@ -3679,7 +3685,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B33" s="33">
         <v>5.9304580792587302E-3</v>
@@ -3701,7 +3707,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B35" s="33">
         <v>5.3690981965173398E-3</v>
@@ -3712,7 +3718,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B36" s="33">
         <v>3.6175072691710698E-3</v>
@@ -3734,7 +3740,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B38" s="33">
         <v>1.2060050678853701E-3</v>
@@ -3745,7 +3751,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B39" s="33">
         <v>1.17362041850181E-3</v>
@@ -3767,7 +3773,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B41" s="33">
         <v>7.6897910828771499E-4</v>
@@ -3778,7 +3784,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B42" s="33">
         <v>1.3113308198388899E-4</v>

</xml_diff>